<commit_message>
Updated NLCD field names
</commit_message>
<xml_diff>
--- a/Docs/FieldNames.xlsx
+++ b/Docs/FieldNames.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="232">
   <si>
     <t>FieldName</t>
   </si>
@@ -315,18 +315,12 @@
     <t>NLCD2</t>
   </si>
   <si>
-    <t>Percent upstream area classified as developed</t>
-  </si>
-  <si>
     <t>NLCD3</t>
   </si>
   <si>
     <t>NLCD4</t>
   </si>
   <si>
-    <t>Percent upstream area classified as forested</t>
-  </si>
-  <si>
     <t>NLCD5</t>
   </si>
   <si>
@@ -336,15 +330,9 @@
     <t>NLCD8</t>
   </si>
   <si>
-    <t>Percent upstream area classified as cultivated</t>
-  </si>
-  <si>
     <t>NLCD9</t>
   </si>
   <si>
-    <t>Percent upstream area classified as wetland</t>
-  </si>
-  <si>
     <t>NLCD11PC</t>
   </si>
   <si>
@@ -441,18 +429,12 @@
     <t>NLCD2_1</t>
   </si>
   <si>
-    <t>Percent catchment area classified as developed</t>
-  </si>
-  <si>
     <t>NLCD3_1</t>
   </si>
   <si>
     <t>NLCD4_1</t>
   </si>
   <si>
-    <t>Percent catchment area classified as forested</t>
-  </si>
-  <si>
     <t>NLCD5_1</t>
   </si>
   <si>
@@ -462,15 +444,9 @@
     <t>NLCD8_1</t>
   </si>
   <si>
-    <t>Percent catchment area classified as cultivated</t>
-  </si>
-  <si>
     <t>NLCD9_1</t>
   </si>
   <si>
-    <t>Percent catchment area classified as wetland</t>
-  </si>
-  <si>
     <t>flooding_SUM</t>
   </si>
   <si>
@@ -691,6 +667,54 @@
   </si>
   <si>
     <t>Percent catchment area that is impervious</t>
+  </si>
+  <si>
+    <t>Upstream area (km2) classified as open water</t>
+  </si>
+  <si>
+    <t>Upstream area (km2) classified as developed</t>
+  </si>
+  <si>
+    <t>Upstream area (km2) classified as barren</t>
+  </si>
+  <si>
+    <t>Upstream area (km2) classified as forested</t>
+  </si>
+  <si>
+    <t>Upstream area (km2) classified as shrubland</t>
+  </si>
+  <si>
+    <t>Upstream area (km2) classified as grassland</t>
+  </si>
+  <si>
+    <t>Upstream area (km2) classified as cultivated</t>
+  </si>
+  <si>
+    <t>Upstream area (km2) classified as wetland</t>
+  </si>
+  <si>
+    <t>Catchment area (km2) classified as open water</t>
+  </si>
+  <si>
+    <t>Catchment area (km2) classified as developed</t>
+  </si>
+  <si>
+    <t>Catchment area (km2) classified as barren</t>
+  </si>
+  <si>
+    <t>Catchment area (km2) classified as forested</t>
+  </si>
+  <si>
+    <t>Catchment area (km2) classified as shrubland</t>
+  </si>
+  <si>
+    <t>Catchment area (km2) classified as grassland</t>
+  </si>
+  <si>
+    <t>Catchment area (km2) classified as cultivated</t>
+  </si>
+  <si>
+    <t>Catchment area (km2) classified as wetland</t>
   </si>
 </sst>
 </file>
@@ -1500,7 +1524,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1897,7 +1923,7 @@
         <v>96</v>
       </c>
       <c r="B49" t="s">
-        <v>67</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1905,535 +1931,535 @@
         <v>97</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B51" t="s">
-        <v>77</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B52" t="s">
-        <v>101</v>
+        <v>219</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>220</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B54" t="s">
-        <v>87</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
-        <v>105</v>
+        <v>222</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B56" t="s">
-        <v>107</v>
+        <v>223</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B57" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B59" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B62" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B64" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B65" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B66" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B67" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B68" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B69" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B70" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B71" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B72" t="s">
-        <v>109</v>
+        <v>224</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B73" t="s">
-        <v>140</v>
+        <v>225</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B74" t="s">
-        <v>119</v>
+        <v>226</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B75" t="s">
-        <v>143</v>
+        <v>227</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B76" t="s">
-        <v>127</v>
+        <v>228</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B77" t="s">
-        <v>129</v>
+        <v>229</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B78" t="s">
-        <v>147</v>
+        <v>230</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B79" t="s">
-        <v>149</v>
+        <v>231</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B80" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B81" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B82" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B83" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B84" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B85" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B86" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B87" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B88" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B89" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B90" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B91" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B92" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B93" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B94" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B95" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B96" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B97" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B98" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B99" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B100" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B101" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B102" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B103" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B104" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B105" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B106" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B107" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B108" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B109" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B110" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B111" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B112" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B113" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B114" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B115" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B116" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>